<commit_message>
updated notebooks, figures and exports
</commit_message>
<xml_diff>
--- a/experiments/2022_car_sampling_pnec/results/descriptive_information.xlsx
+++ b/experiments/2022_car_sampling_pnec/results/descriptive_information.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10708"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/HealthPsychology/CARWatch/Code/carwatch_analysis/experiments/2022_car_sampling_pnec/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8B6615-DB8F-FB42-9865-BF6908425BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22400" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Age" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
     <sheet name="Log_Type_Statistics" sheetId="4" r:id="rId4"/>
     <sheet name="CAR" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -107,8 +101,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,11 +154,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -174,14 +165,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -228,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,27 +243,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,24 +277,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,14 +452,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,7 +475,7 @@
         <v>24.23076923076923</v>
       </c>
       <c r="C2">
-        <v>8.6479892876349691</v>
+        <v>8.647989287634969</v>
       </c>
     </row>
   </sheetData>
@@ -537,14 +484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -555,7 +502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -563,10 +510,10 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>0.20512820512820509</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.2051282051282051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -574,7 +521,7 @@
         <v>93</v>
       </c>
       <c r="C3">
-        <v>0.79487179487179482</v>
+        <v>0.7948717948717948</v>
       </c>
     </row>
   </sheetData>
@@ -583,14 +530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -604,8 +551,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -615,11 +562,11 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>0.15492957746478869</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+        <v>0.1549295774647887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -627,11 +574,11 @@
         <v>60</v>
       </c>
       <c r="D3">
-        <v>0.84507042253521125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+        <v>0.8450704225352113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -644,8 +591,8 @@
         <v>0.2181818181818182</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -653,11 +600,11 @@
         <v>86</v>
       </c>
       <c r="D5">
-        <v>0.78181818181818186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+        <v>0.7818181818181819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -670,8 +617,8 @@
         <v>0.2452830188679245</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -679,7 +626,7 @@
         <v>40</v>
       </c>
       <c r="D7">
-        <v>0.75471698113207553</v>
+        <v>0.7547169811320755</v>
       </c>
     </row>
   </sheetData>
@@ -693,19 +640,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="209" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -716,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -727,7 +669,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -738,7 +680,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -749,7 +691,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -760,7 +702,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -771,7 +713,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -782,7 +724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -793,7 +735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -804,7 +746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -821,16 +763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="287" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,18 +781,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B2">
-        <v>123.33891413122571</v>
+        <v>123.34</v>
       </c>
       <c r="C2">
-        <v>182.55872947321359</v>
+        <v>182.56</v>
       </c>
       <c r="D2">
-        <v>12.781667652339911</v>
+        <v>12.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed everything from "log type" to "reporting type"
changed sampling delay from \Delta s to \Delta t
</commit_message>
<xml_diff>
--- a/experiments/2022_car_sampling_pnec/results/descriptive_information.xlsx
+++ b/experiments/2022_car_sampling_pnec/results/descriptive_information.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/HealthPsychology/CARWatch/Code/carwatch_analysis/experiments/2022_car_sampling_pnec/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC65DC-6D07-F044-A541-08A8AAEB48A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Age" sheetId="1" r:id="rId1"/>
     <sheet name="Gender_Total" sheetId="2" r:id="rId2"/>
     <sheet name="Gender_Conditions" sheetId="3" r:id="rId3"/>
-    <sheet name="Log_Type_Statistics" sheetId="4" r:id="rId4"/>
+    <sheet name="Reporting_Type_Statistics" sheetId="4" r:id="rId4"/>
     <sheet name="CAR" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -68,7 +62,7 @@
     <t>nights</t>
   </si>
   <si>
-    <t>log_type</t>
+    <t>reporting_type</t>
   </si>
   <si>
     <t>Naive</t>
@@ -107,8 +101,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,11 +154,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -174,14 +165,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -228,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,27 +243,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,24 +277,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,14 +452,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,7 +475,7 @@
         <v>24.23076923076923</v>
       </c>
       <c r="C2">
-        <v>8.6479892876349691</v>
+        <v>8.647989287634969</v>
       </c>
     </row>
   </sheetData>
@@ -537,14 +484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -555,7 +502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -563,10 +510,10 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>0.20512820512820509</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.2051282051282051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -574,7 +521,7 @@
         <v>93</v>
       </c>
       <c r="C3">
-        <v>0.79487179487179482</v>
+        <v>0.7948717948717948</v>
       </c>
     </row>
   </sheetData>
@@ -583,14 +530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -604,8 +551,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -615,11 +562,11 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>0.15492957746478869</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+        <v>0.1549295774647887</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -627,11 +574,11 @@
         <v>60</v>
       </c>
       <c r="D3">
-        <v>0.84507042253521125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+        <v>0.8450704225352113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -644,8 +591,8 @@
         <v>0.2181818181818182</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -653,11 +600,11 @@
         <v>86</v>
       </c>
       <c r="D5">
-        <v>0.78181818181818186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+        <v>0.7818181818181819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -670,8 +617,8 @@
         <v>0.2452830188679245</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -679,7 +626,7 @@
         <v>40</v>
       </c>
       <c r="D7">
-        <v>0.75471698113207553</v>
+        <v>0.7547169811320755</v>
       </c>
     </row>
   </sheetData>
@@ -693,19 +640,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -716,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -727,7 +669,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -738,7 +680,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -749,7 +691,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -760,7 +702,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -771,7 +713,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -782,7 +724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -793,7 +735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -804,7 +746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -821,14 +763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>